<commit_message>
commiting till linked list 3rd question of binary to int
</commit_message>
<xml_diff>
--- a/excel/Fraz.xlsx
+++ b/excel/Fraz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chinmay panchal\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chinmay panchal\OneDrive\Documents\fraz Dsa sheet\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839A61C2-9761-47A3-AF35-B9F6977F3691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AA363C-6F27-4C54-918C-931229AEE9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C1FB8044-A3FD-4964-AC4F-B7AA64F9F631}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
   <si>
     <t>array</t>
   </si>
@@ -211,6 +211,60 @@
   </si>
   <si>
     <t>sign integer overflow error mai longlong int lena h, log(underroot of x) time complexity agar mid*mid&lt;=x h toh ans = mid and s = mid otherwise e = mid-1;</t>
+  </si>
+  <si>
+    <t>recursion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power of 2 </t>
+  </si>
+  <si>
+    <t>2 se modulo bhi hona chahiye aur uske baad wala bhi 2 se modulo hona chahiye kyunki 2*2*2….. Asia hi hoga and base case true if  n==1 and false  when n == 0;</t>
+  </si>
+  <si>
+    <t>pow (x,n)</t>
+  </si>
+  <si>
+    <t>dekho yaar agar n&lt;0 h toh pehle x = 1/x , kardo and n ka abs kardo so who positive jojayega now agar n odd h toh x*fun(x*x,n/2) and even h toh fun(x*x,n/2);  aur base case toh n==0 || x==1 return 1 and x=0 toh 0</t>
+  </si>
+  <si>
+    <t>reverse a linked list</t>
+  </si>
+  <si>
+    <t>prev = null , curr = null agar head != NULL h toh curr = head-&gt;next; then jab tak curr null nahi hojata loop chalao aur recursion mai head-&gt;next = null, haed-&gt;next-&gt;next = head; aur first mai anshead = reverse(h-&gt;n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">merge two sorted </t>
+  </si>
+  <si>
+    <t>ab recursion se kasie karna h nahi pata</t>
+  </si>
+  <si>
+    <t>reverse a string</t>
+  </si>
+  <si>
+    <t>kuch nai wohi h yaar ki bas base case dekhna hota h i&gt;=j h toh return aur swap and I+1 and j-1  that's  it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked list </t>
+  </si>
+  <si>
+    <t>delete node</t>
+  </si>
+  <si>
+    <t>kuch nahi h value change kardo aur next wale ko delete kardo ek hi baat h</t>
+  </si>
+  <si>
+    <t>find middle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bruteforce ( size count karo aur fir bas ) = slow fast dono barabar hi h yaar kuch khas diff yahi h ki isme likha kam ha aisa </t>
+  </si>
+  <si>
+    <t>binary to integer</t>
+  </si>
+  <si>
+    <t>bruteforce size nikalo and size - 1 carry hojayega agar 1 aaya toh 2 ki power carry + ans = ans; aur ek aur way h ki ans = ans * 2 + head-&gt;val;</t>
   </si>
 </sst>
 </file>
@@ -562,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FD4609-E510-408D-98FF-94D481501BBE}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -860,6 +914,95 @@
         <v>17</v>
       </c>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>